<commit_message>
Update region xls files.
</commit_message>
<xml_diff>
--- a/pp/files/samples/xls/region_sample.xlsx
+++ b/pp/files/samples/xls/region_sample.xlsx
@@ -6137,7 +6137,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>values!$B$2:$B$10</xm:f>
@@ -6148,7 +6148,7 @@
           <x14:formula1>
             <xm:f>region_codes!$A$2:$A$252</xm:f>
           </x14:formula1>
-          <xm:sqref>B10:B104</xm:sqref>
+          <xm:sqref>B2:B104</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -6168,12 +6168,6 @@
           </x14:formula1>
           <xm:sqref>V2:V104</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]region_codes!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B9</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -6185,8 +6179,8 @@
   <dimension ref="A1:C252"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A222" sqref="A222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>

</xml_diff>